<commit_message>
Thurs 17th Dec - import + PEP8 compliance
</commit_message>
<xml_diff>
--- a/create-data/create_reference_data/source/additional_code_types/additional_code_types.xlsx
+++ b/create-data/create_reference_data/source/additional_code_types/additional_code_types.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt.admin/projects/tariffs/create-data/create_reference_data/source/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt.admin/projects/tariffs/create-data/create_reference_data/source/additional_code_types/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFBFD6E-4F5F-7A46-951F-377F7E892341}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0EAB440-DCC9-DD43-A000-08545F09654C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16180" windowHeight="9560" xr2:uid="{B724F9FD-527C-4A95-969C-B8CCC70DC96A}"/>
+    <workbookView xWindow="20740" yWindow="4660" windowWidth="14480" windowHeight="9560" xr2:uid="{B724F9FD-527C-4A95-969C-B8CCC70DC96A}"/>
   </bookViews>
   <sheets>
     <sheet name="Updated" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -56,6 +56,12 @@
   </si>
   <si>
     <t>APPLICATION_CODE</t>
+  </si>
+  <si>
+    <t>Prohibition / restriction /  surveillance</t>
+  </si>
+  <si>
+    <t>Export refunds</t>
   </si>
 </sst>
 </file>
@@ -433,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E5B35DA-628F-40A1-97BB-3E7F8D8C3603}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -484,6 +490,22 @@
       </c>
       <c r="B5" s="4" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>9</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>